<commit_message>
Created sprint 2 backlog
Created sprint 2 backlog
Updated product backlog
</commit_message>
<xml_diff>
--- a/Product Backlog/Product Backlog.xlsx
+++ b/Product Backlog/Product Backlog.xlsx
@@ -51,9 +51,6 @@
     <t>As a developer I want to be able to update the database</t>
   </si>
   <si>
-    <t>As a developer, I want my web app to meet WCAG accessibility standards</t>
-  </si>
-  <si>
     <t>As a developer, I want a host for the web app</t>
   </si>
   <si>
@@ -85,13 +82,16 @@
   </si>
   <si>
     <t>As a user, I can sort results using a custom ranking algorithm baased on a combination of price and distance</t>
+  </si>
+  <si>
+    <t>As a user, I want a more user friendly website</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -102,8 +102,14 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +120,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC9DAF8"/>
         <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -129,17 +141,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,8 +378,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -386,54 +404,54 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2">
+      <c r="C2" s="4">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <f>C2/D2</f>
         <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
+      <c r="B3" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="C3" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E14" si="0">C3/D3</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>13</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>0.76923076923076927</v>
       </c>
@@ -442,16 +460,16 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>9</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -459,7 +477,7 @@
     <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>
@@ -474,24 +492,24 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="2">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
@@ -506,24 +524,24 @@
     </row>
     <row r="9" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4">
         <v>7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="2">
         <v>5</v>
@@ -540,32 +558,32 @@
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4">
         <v>10</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>5</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -574,8 +592,8 @@
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
+      <c r="B13" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="2">
         <v>5</v>
@@ -590,8 +608,8 @@
     </row>
     <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
+      <c r="B14" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C14" s="2">
         <v>5</v>
@@ -609,5 +627,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>